<commit_message>
Question with Image - Upload-Fix
</commit_message>
<xml_diff>
--- a/excelTemplate/Frage_Template_de.xlsx
+++ b/excelTemplate/Frage_Template_de.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -10,8 +10,8 @@
     <sheet name="Frage-Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Antwortmöglichkeiten">'Frage-Template'!$C$2:$K$2</definedName>
-    <definedName name="Fragetypen">'Frage-Template'!$N$2:$N$8</definedName>
+    <definedName name="Antwortmöglichkeiten">'Frage-Template'!$D$2:$L$2</definedName>
+    <definedName name="Fragetypen">'Frage-Template'!$O$2:$O$8</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Frage</t>
   </si>
@@ -177,6 +177,28 @@
   </si>
   <si>
     <t>[img=Logo5.jpg]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Frage-Bild
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Muss sich im gleichen Ordner wie diese Datei befinden.</t>
+    </r>
+  </si>
+  <si>
+    <t>bits.png</t>
+  </si>
+  <si>
+    <t>prog-lang.jpg</t>
   </si>
 </sst>
 </file>
@@ -371,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,6 +477,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,31 +803,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="46.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
-    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.77734375" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
@@ -810,9 +836,11 @@
         <v>0</v>
       </c>
       <c r="C1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
@@ -820,52 +848,54 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
       <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="N1" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="28"/>
+      <c r="O1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="19"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -874,66 +904,70 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
-      <c r="N3" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="O3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="8"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="N4" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="O4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="8"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="11"/>
-      <c r="N5" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="11"/>
+      <c r="O5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="21"/>
-      <c r="C6" s="8"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="11"/>
-      <c r="N6" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="11"/>
+      <c r="O6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="9"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -942,46 +976,49 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
-      <c r="N7" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+      <c r="O7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="11"/>
-      <c r="N8" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="11"/>
+      <c r="O8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="8"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K9" s="9"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="20"/>
-      <c r="C10" s="8"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -990,12 +1027,13 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="8"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1004,12 +1042,13 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L11" s="8"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="21"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1018,12 +1057,13 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L12" s="8"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1032,12 +1072,13 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L13" s="8"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1046,12 +1087,13 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L14" s="8"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="8"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1060,12 +1102,13 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L15" s="8"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="20"/>
-      <c r="C16" s="8"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1074,12 +1117,13 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L16" s="8"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1088,12 +1132,13 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="8"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="20"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1102,12 +1147,13 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="8"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18"/>
       <c r="B19" s="22"/>
-      <c r="C19" s="12"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -1116,9 +1162,10 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L19" s="12"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1131,11 +1178,12 @@
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="8"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1145,16 +1193,17 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="14"/>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -1163,38 +1212,42 @@
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="6">
         <v>1</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6">
         <v>3</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6">
         <v>10</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6">
+      <c r="I23" s="6"/>
+      <c r="J23" s="6">
         <v>8</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="K23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="6">
+      <c r="L23" s="6">
         <v>7</v>
       </c>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>7</v>
       </c>
@@ -1202,89 +1255,94 @@
         <v>14</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="9" t="s">
+      <c r="K24" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="10"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L24" s="8"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="9"/>
+      <c r="J25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="9"/>
+      <c r="L25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="F26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="H26" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="9"/>
+      <c r="J26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="11"/>
-    </row>
-    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K26" s="9"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>10</v>
       </c>
@@ -1299,71 +1357,75 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="10"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K27" s="9"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8"/>
+      <c r="F28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="11"/>
-    </row>
-    <row r="29" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="9"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="24"/>
+      <c r="D29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="24"/>
+      <c r="H29" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="24"/>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="24"/>
+      <c r="J29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="24"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="13"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="13"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A23:A1048576 A3:A19">

</xml_diff>

<commit_message>
updated execlTemplate to only show supported types
</commit_message>
<xml_diff>
--- a/excelTemplate/Frage_Template_de.xlsx
+++ b/excelTemplate/Frage_Template_de.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Frage</t>
   </si>
@@ -53,15 +53,6 @@
   </si>
   <si>
     <t>Multiplechoice Bilder</t>
-  </si>
-  <si>
-    <t>Freitext</t>
-  </si>
-  <si>
-    <t>Lückentext</t>
-  </si>
-  <si>
-    <t>Drag und Drop</t>
   </si>
   <si>
     <t>Wie viele Bits ergeben 1 Byte?</t>
@@ -104,24 +95,6 @@
     <t>Welches sind Micosoft Office - Programme?</t>
   </si>
   <si>
-    <t>Welches ist Programmiersprache ist deiner Meinung nach die Beste?</t>
-  </si>
-  <si>
-    <t>Freeware</t>
-  </si>
-  <si>
-    <t>Gratissoftware</t>
-  </si>
-  <si>
-    <t>Gratis-Software</t>
-  </si>
-  <si>
-    <t>Ordne die Programme dem Hersteller zu.</t>
-  </si>
-  <si>
-    <t>Eine * ist ein kostenloses Programm für den Computer.</t>
-  </si>
-  <si>
     <t>Drag-Item; Drop-Location</t>
   </si>
   <si>
@@ -137,9 +110,6 @@
     <t>Beispiele</t>
   </si>
   <si>
-    <t>[img=Word.jpg]; [img=Microsoft.jpg]</t>
-  </si>
-  <si>
     <t>[img=Logo1.jpg]</t>
   </si>
   <si>
@@ -150,15 +120,6 @@
   </si>
   <si>
     <t>[img=Logo4.jpg]</t>
-  </si>
-  <si>
-    <t>iOS; Apple</t>
-  </si>
-  <si>
-    <t>Android; [img=Google.jpg]</t>
-  </si>
-  <si>
-    <t>[img=HSR_Mapper.png]; HSR</t>
   </si>
   <si>
     <t>[img=Powerpoint.jpg]</t>
@@ -803,10 +764,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +786,7 @@
     <col min="12" max="12" width="21.77734375" customWidth="1"/>
     <col min="13" max="13" width="6.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -836,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
@@ -851,7 +812,7 @@
       <c r="L1" s="27"/>
       <c r="M1" s="28"/>
       <c r="O1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -862,31 +823,31 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
         <v>6</v>
@@ -960,9 +921,6 @@
       <c r="K6" s="9"/>
       <c r="L6" s="8"/>
       <c r="M6" s="11"/>
-      <c r="O6" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
@@ -978,9 +936,6 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="10"/>
-      <c r="O7" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -996,9 +951,6 @@
       <c r="K8" s="9"/>
       <c r="L8" s="8"/>
       <c r="M8" s="11"/>
-      <c r="O8" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
@@ -1197,12 +1149,12 @@
     </row>
     <row r="22" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1219,10 +1171,10 @@
         <v>6</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -1240,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="L23" s="6">
         <v>7</v>
@@ -1252,30 +1204,30 @@
         <v>7</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="10"/>
@@ -1285,140 +1237,69 @@
         <v>8</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="8" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="M25" s="11"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="F26" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="9"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="11"/>
-    </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="11"/>
-    </row>
-    <row r="29" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="24"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="24"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="L27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1428,8 +1309,8 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A23:A1048576 A3:A19">
-      <formula1>Fragetypen</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A19 A27:A1048576">
+      <formula1>$O$2:$O$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>